<commit_message>
Added gitignore and included .asv and .mat
</commit_message>
<xml_diff>
--- a/Sag_fault_calculation/line_data.xlsx
+++ b/Sag_fault_calculation/line_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kople\Documents\Personal Git repos\UM-coursework\Sag_fault_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93272297-5A7E-426D-B559-477F14B597E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A351D-EC99-4FB2-99E6-5CEA24397548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3828" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Calculated average sags at lines
</commit_message>
<xml_diff>
--- a/Sag_fault_calculation/line_data.xlsx
+++ b/Sag_fault_calculation/line_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kople\Documents\Personal Git repos\UM-coursework\Sag_fault_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A351D-EC99-4FB2-99E6-5CEA24397548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFBDA56-893D-4A19-B73E-93B1470C7864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>